<commit_message>
code commit for checking
</commit_message>
<xml_diff>
--- a/business_logic/excel_extracter/Test_Excel_Data_Extr/output_file.xlsx
+++ b/business_logic/excel_extracter/Test_Excel_Data_Extr/output_file.xlsx
@@ -440,7 +440,7 @@
     <col width="103" customWidth="1" min="1" max="1"/>
     <col width="12" customWidth="1" min="2" max="2"/>
     <col width="12" customWidth="1" min="3" max="3"/>
-    <col width="93" customWidth="1" min="4" max="4"/>
+    <col width="62" customWidth="1" min="4" max="4"/>
     <col width="12" customWidth="1" min="5" max="5"/>
     <col width="12" customWidth="1" min="6" max="6"/>
     <col width="16" customWidth="1" min="7" max="7"/>
@@ -449,7 +449,7 @@
     <col width="12" customWidth="1" min="10" max="10"/>
     <col width="13" customWidth="1" min="11" max="11"/>
     <col width="15" customWidth="1" min="12" max="12"/>
-    <col width="19" customWidth="1" min="13" max="13"/>
+    <col width="13" customWidth="1" min="13" max="13"/>
     <col width="21" customWidth="1" min="14" max="14"/>
     <col width="13" customWidth="1" min="15" max="15"/>
   </cols>
@@ -630,7 +630,7 @@
         </is>
       </c>
       <c r="N6" s="2" t="n">
-        <v>45324</v>
+        <v>45232</v>
       </c>
       <c r="O6" t="inlineStr"/>
     </row>
@@ -644,7 +644,7 @@
       <c r="C7" t="inlineStr"/>
       <c r="D7" t="inlineStr">
         <is>
-          <t>OPTIMUM AUTOS</t>
+          <t>TP WATERS</t>
         </is>
       </c>
       <c r="E7" t="inlineStr"/>
@@ -662,7 +662,7 @@
       </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t>IREN240202-1</t>
+          <t>IREN231102-1</t>
         </is>
       </c>
       <c r="O7" t="inlineStr"/>
@@ -673,7 +673,7 @@
       <c r="C8" t="inlineStr"/>
       <c r="D8" t="inlineStr">
         <is>
-          <t>APPLEGREEN PETROL STATAION DARRAGH KILRUSH ROAD ENNIS V95RR97 CO. CLARE, IRELAND</t>
+          <t>MONASTEREVIN RD, KILNAGORNAN, CO. KILDARE, R51 EV29, IRELAND</t>
         </is>
       </c>
       <c r="E8" t="inlineStr"/>
@@ -694,7 +694,7 @@
       <c r="C9" t="inlineStr"/>
       <c r="D9" t="inlineStr">
         <is>
-          <t>(PH) 353 851353950 / (EMAIL) OPTIMUMCARSALES@GMAIL.COM</t>
+          <t>(PH) 353 85 386 6717 / (Email) marie@tpwaters.ie’</t>
         </is>
       </c>
       <c r="E9" t="inlineStr"/>
@@ -719,7 +719,7 @@
       <c r="C10" t="inlineStr"/>
       <c r="D10" t="inlineStr">
         <is>
-          <t>IPS GROUP</t>
+          <t>SAME AS CONSIGNEE</t>
         </is>
       </c>
       <c r="E10" t="inlineStr"/>
@@ -738,11 +738,7 @@
       <c r="A11" t="inlineStr"/>
       <c r="B11" t="inlineStr"/>
       <c r="C11" t="inlineStr"/>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>IPS GROUPAGE SERVICES LTD., UNIT 102 DONNYBROOK COMMERCIAL CENTRE,  DOUGLAS,  CORK IRELAND.</t>
-        </is>
-      </c>
+      <c r="D11" t="inlineStr"/>
       <c r="E11" t="inlineStr"/>
       <c r="F11" t="inlineStr"/>
       <c r="G11" t="inlineStr"/>
@@ -759,11 +755,7 @@
       <c r="A12" t="inlineStr"/>
       <c r="B12" t="inlineStr"/>
       <c r="C12" t="inlineStr"/>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>(PH) 353 21 4895777 / (EMAIL) JOE@IPS-GROUP.COM</t>
-        </is>
-      </c>
+      <c r="D12" t="inlineStr"/>
       <c r="E12" t="inlineStr"/>
       <c r="F12" t="inlineStr"/>
       <c r="G12" t="inlineStr"/>
@@ -912,46 +904,46 @@
         <v>1</v>
       </c>
       <c r="E17" t="n">
-        <v>2013</v>
+        <v>2018</v>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>AUDI</t>
+          <t>VOLKSWAGEN</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>A1 SPORTBACK</t>
+          <t>GOLF</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>264338</t>
+          <t>257434</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>WAUZZZ8XXDB086170</t>
+          <t>WVWZZZAUZJW276698</t>
         </is>
       </c>
       <c r="J17" t="n">
-        <v>1220</v>
+        <v>1240</v>
       </c>
       <c r="K17" t="n">
-        <v>3.97</v>
+        <v>4.26</v>
       </c>
       <c r="L17" t="n">
-        <v>1.74</v>
+        <v>1.8</v>
       </c>
       <c r="M17" t="n">
-        <v>1.44</v>
+        <v>1.48</v>
       </c>
       <c r="N17" t="n">
-        <v>9.946999999999999</v>
+        <v>11.349</v>
       </c>
       <c r="O17" t="inlineStr">
         <is>
-          <t>1400 CC</t>
+          <t>1200 CC</t>
         </is>
       </c>
     </row>
@@ -963,46 +955,46 @@
         <v>2</v>
       </c>
       <c r="E18" t="n">
-        <v>2016</v>
+        <v>2018</v>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>VOLKSWAGEN</t>
+          <t>MAZDA</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>GOLF</t>
+          <t>DEMIO</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>264488</t>
+          <t>257667</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>WVWZZZAUZGW153858</t>
+          <t>DJ3FS-518869</t>
         </is>
       </c>
       <c r="J18" t="n">
-        <v>1240</v>
+        <v>1030</v>
       </c>
       <c r="K18" t="n">
-        <v>4.26</v>
+        <v>4.06</v>
       </c>
       <c r="L18" t="n">
-        <v>1.8</v>
+        <v>1.69</v>
       </c>
       <c r="M18" t="n">
-        <v>1.48</v>
+        <v>1.5</v>
       </c>
       <c r="N18" t="n">
-        <v>11.349</v>
+        <v>10.292</v>
       </c>
       <c r="O18" t="inlineStr">
         <is>
-          <t>1200 CC</t>
+          <t>1300 CC</t>
         </is>
       </c>
     </row>
@@ -1014,46 +1006,46 @@
         <v>3</v>
       </c>
       <c r="E19" t="n">
-        <v>2016</v>
+        <v>2017</v>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>AUDI</t>
+          <t>VOLKSWAGEN</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>A3 SPORTBACK</t>
+          <t>GOLF</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>264711</t>
+          <t>259249</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>WAUZZZ8V9GA172515</t>
+          <t>WVWZZZAUZJW045727</t>
         </is>
       </c>
       <c r="J19" t="n">
-        <v>1320</v>
+        <v>1240</v>
       </c>
       <c r="K19" t="n">
-        <v>4.32</v>
+        <v>4.26</v>
       </c>
       <c r="L19" t="n">
-        <v>1.78</v>
+        <v>1.8</v>
       </c>
       <c r="M19" t="n">
-        <v>1.46</v>
+        <v>1.48</v>
       </c>
       <c r="N19" t="n">
-        <v>11.227</v>
+        <v>11.349</v>
       </c>
       <c r="O19" t="inlineStr">
         <is>
-          <t>1400 CC</t>
+          <t>1200 CC</t>
         </is>
       </c>
     </row>
@@ -1065,46 +1057,46 @@
         <v>4</v>
       </c>
       <c r="E20" t="n">
-        <v>2014</v>
+        <v>2018</v>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>MERCEDES</t>
+          <t>VOLKSWAGEN</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>A180</t>
+          <t>GOLF</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>264940</t>
+          <t>259997</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>WDD1760422V034989</t>
+          <t>WVWZZZAUZJW296218</t>
         </is>
       </c>
       <c r="J20" t="n">
-        <v>1440</v>
+        <v>1240</v>
       </c>
       <c r="K20" t="n">
-        <v>4.35</v>
+        <v>4.26</v>
       </c>
       <c r="L20" t="n">
-        <v>1.78</v>
+        <v>1.8</v>
       </c>
       <c r="M20" t="n">
-        <v>1.42</v>
+        <v>1.48</v>
       </c>
       <c r="N20" t="n">
-        <v>10.995</v>
+        <v>11.349</v>
       </c>
       <c r="O20" t="inlineStr">
         <is>
-          <t>1600 CC</t>
+          <t>1200 CC</t>
         </is>
       </c>
     </row>
@@ -1116,46 +1108,46 @@
         <v>5</v>
       </c>
       <c r="E21" t="n">
-        <v>2014</v>
+        <v>2018</v>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>MERCEDES</t>
+          <t>VOLKSWAGEN</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>A180</t>
+          <t>POLO</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>265343</t>
+          <t>262279</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>WDD1760422V030026</t>
+          <t>WVWZZZAWZJU028693</t>
         </is>
       </c>
       <c r="J21" t="n">
-        <v>1440</v>
+        <v>1160</v>
       </c>
       <c r="K21" t="n">
-        <v>4.35</v>
+        <v>4.06</v>
       </c>
       <c r="L21" t="n">
-        <v>1.78</v>
+        <v>1.75</v>
       </c>
       <c r="M21" t="n">
-        <v>1.42</v>
+        <v>1.45</v>
       </c>
       <c r="N21" t="n">
-        <v>10.995</v>
+        <v>10.302</v>
       </c>
       <c r="O21" t="inlineStr">
         <is>
-          <t>1600 CC</t>
+          <t>990 CC</t>
         </is>
       </c>
     </row>
@@ -1179,7 +1171,7 @@
       </c>
       <c r="H22" t="inlineStr"/>
       <c r="I22" t="n">
-        <v>6660</v>
+        <v>5910</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
@@ -1189,7 +1181,7 @@
       <c r="K22" t="inlineStr"/>
       <c r="L22" t="inlineStr"/>
       <c r="M22" t="n">
-        <v>54.51299999999999</v>
+        <v>54.641</v>
       </c>
       <c r="N22" t="inlineStr">
         <is>
@@ -1224,7 +1216,7 @@
       <c r="F24" t="inlineStr"/>
       <c r="G24" t="inlineStr">
         <is>
-          <t>EBKG07870938</t>
+          <t>EBKG07048809</t>
         </is>
       </c>
       <c r="H24" t="inlineStr"/>
@@ -1304,7 +1296,7 @@
       <c r="C27" t="inlineStr"/>
       <c r="D27" t="inlineStr">
         <is>
-          <t>MSC MONTEREY</t>
+          <t>MSC NAGOYA V</t>
         </is>
       </c>
       <c r="E27" t="inlineStr"/>
@@ -1333,7 +1325,7 @@
       <c r="C28" t="inlineStr"/>
       <c r="D28" t="inlineStr">
         <is>
-          <t>NO.HI407A</t>
+          <t>NO.HI346A</t>
         </is>
       </c>
       <c r="E28" t="inlineStr"/>
@@ -1365,7 +1357,7 @@
       <c r="B29" t="inlineStr"/>
       <c r="C29" t="inlineStr"/>
       <c r="D29" s="2" t="n">
-        <v>45337</v>
+        <v>45246</v>
       </c>
       <c r="E29" t="inlineStr"/>
       <c r="F29" t="inlineStr"/>

</xml_diff>